<commit_message>
Changed 'drag to bin' to select and delete for removing nodes. Created if-else node.
</commit_message>
<xml_diff>
--- a/RegexNodes/Node Colors.xlsx
+++ b/RegexNodes/Node Colors.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8b061eb7d1723a09/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Files\Visual Studio\RegexNodes\RegexNodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D97087A0-72DA-413E-A074-1D7A35D75667}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2291CA-6462-4D4F-800A-0BA07FF8B99C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{5B264E41-D4A5-4A76-B5FF-950409F1D3C6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>Mult:</t>
   </si>
@@ -91,6 +91,54 @@
   </si>
   <si>
     <t>80%</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>wildcard</t>
+  </si>
+  <si>
+    <t>characterset</t>
+  </si>
+  <si>
+    <t>anchor</t>
+  </si>
+  <si>
+    <t>whitespace</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>concatenate</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>quantifier</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>lookaround</t>
+  </si>
+  <si>
+    <t>if-else</t>
+  </si>
+  <si>
+    <t>flags</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>70%</t>
   </si>
 </sst>
 </file>
@@ -449,7 +497,7 @@
   <dimension ref="C3:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,8 +522,8 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f>360/15</f>
-        <v>24</v>
+        <f>360/16</f>
+        <v>22.5</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -491,11 +539,11 @@
         <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="K4" t="str">
-        <f>J4&amp;" hsl("&amp;ROUND(F4,0)&amp;","&amp;G4&amp;", "&amp;H4&amp;");"</f>
-        <v xml:space="preserve">    --col-node-anchor: hsl(0,80%, 75%);</v>
+        <f>"--col-node-"&amp;J4&amp;": hsl("&amp;ROUND(F4,0)&amp;","&amp;G4&amp;", "&amp;H4&amp;");"</f>
+        <v>--col-node-text: hsl(0,80%, 75%);</v>
       </c>
       <c r="O4" t="s">
         <v>1</v>
@@ -507,7 +555,7 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5:F17" si="0">(E5-1)*$D$4</f>
-        <v>24</v>
+        <v>22.5</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>19</v>
@@ -516,11 +564,11 @@
         <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K17" si="1">J5&amp;" hsl("&amp;ROUND(F5,0)&amp;","&amp;G5&amp;", "&amp;H5&amp;");"</f>
-        <v xml:space="preserve">    --col-node-characterset: hsl(24,80%, 75%);</v>
+        <f t="shared" ref="K5:K18" si="1">"--col-node-"&amp;J5&amp;": hsl("&amp;ROUND(F5,0)&amp;","&amp;G5&amp;", "&amp;H5&amp;");"</f>
+        <v>--col-node-wildcard: hsl(23,80%, 75%);</v>
       </c>
       <c r="O5" t="s">
         <v>2</v>
@@ -532,7 +580,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>19</v>
@@ -541,11 +589,11 @@
         <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-comment: hsl(48,80%, 75%);</v>
+        <v>--col-node-characterset: hsl(45,80%, 75%);</v>
       </c>
       <c r="O6" t="s">
         <v>3</v>
@@ -557,7 +605,7 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>67.5</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>19</v>
@@ -566,11 +614,11 @@
         <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-concatenate: hsl(72,80%, 75%);</v>
+        <v>--col-node-anchor: hsl(68,80%, 75%);</v>
       </c>
       <c r="O7" t="s">
         <v>4</v>
@@ -582,7 +630,7 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>19</v>
@@ -591,11 +639,11 @@
         <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-flags: hsl(96,80%, 75%);</v>
+        <v>--col-node-whitespace: hsl(90,80%, 75%);</v>
       </c>
       <c r="O8" t="s">
         <v>5</v>
@@ -607,7 +655,7 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>112.5</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>19</v>
@@ -616,11 +664,11 @@
         <v>18</v>
       </c>
       <c r="J9" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-group:  hsl(120,80%, 75%);</v>
+        <v>--col-node-comment: hsl(113,80%, 75%);</v>
       </c>
       <c r="O9" t="s">
         <v>6</v>
@@ -632,7 +680,7 @@
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>19</v>
@@ -641,11 +689,11 @@
         <v>18</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-lookaround: hsl(144,80%, 75%);</v>
+        <v>--col-node-or: hsl(135,80%, 75%);</v>
       </c>
       <c r="O10" t="s">
         <v>7</v>
@@ -657,7 +705,7 @@
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>168</v>
+        <v>157.5</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>19</v>
@@ -666,11 +714,11 @@
         <v>18</v>
       </c>
       <c r="J11" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-or: hsl(168,80%, 75%);</v>
+        <v>--col-node-concatenate: hsl(158,80%, 75%);</v>
       </c>
       <c r="O11" t="s">
         <v>8</v>
@@ -682,7 +730,7 @@
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>19</v>
@@ -691,11 +739,11 @@
         <v>18</v>
       </c>
       <c r="J12" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-output: hsl(192,80%, 75%);</v>
+        <v>--col-node-group: hsl(180,80%, 75%);</v>
       </c>
       <c r="O12" t="s">
         <v>9</v>
@@ -707,7 +755,7 @@
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>216</v>
+        <v>202.5</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>19</v>
@@ -716,11 +764,11 @@
         <v>18</v>
       </c>
       <c r="J13" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-quantifier: hsl(216,80%, 75%);</v>
+        <v>--col-node-quantifier: hsl(203,80%, 75%);</v>
       </c>
       <c r="O13" t="s">
         <v>10</v>
@@ -732,7 +780,7 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>19</v>
@@ -741,11 +789,11 @@
         <v>18</v>
       </c>
       <c r="J14" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-reference: hsl(240,80%, 75%);</v>
+        <v>--col-node-reference: hsl(225,80%, 75%);</v>
       </c>
       <c r="O14" t="s">
         <v>11</v>
@@ -757,20 +805,20 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>264</v>
+        <v>247.5</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="J15" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-text: hsl(264,80%, 75%);</v>
+        <v>--col-node-lookaround: hsl(248,80%, 70%);</v>
       </c>
       <c r="O15" t="s">
         <v>12</v>
@@ -782,20 +830,20 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="J16" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-whitespace: hsl(288,80%, 75%);</v>
+        <v>--col-node-if-else: hsl(270,80%, 70%);</v>
       </c>
       <c r="O16" t="s">
         <v>13</v>
@@ -807,27 +855,46 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>312</v>
+        <v>292.5</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="J17" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    --col-node-wildcard: hsl(312,80%, 75%);</v>
+        <v>--col-node-flags: hsl(293,80%, 70%);</v>
       </c>
       <c r="O17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="F18" s="1"/>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1">
+        <f>(E18-1)*$D$4</f>
+        <v>315</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>--col-node-output: hsl(315,80%, 75%);</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J4:J17">
@@ -836,7 +903,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="H5:H17 H4" numberStoredAsText="1"/>
+    <ignoredError sqref="H5:H14 H4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>